<commit_message>
✨ modify code for b2b
</commit_message>
<xml_diff>
--- a/data/dataset_rag_zurich.xlsx
+++ b/data/dataset_rag_zurich.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maicolrodrigues/Documents/Test/Insurapolis/chatbot/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A539515-B543-B44A-B640-73613F0FC979}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0976D99-BC21-7F44-BDD5-D0524D412285}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="50040" yWindow="-9420" windowWidth="47140" windowHeight="26400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -387,65 +387,6 @@
   </si>
   <si>
     <t>Art. 402, 404</t>
-  </si>
-  <si>
-    <t>Art.403 Supervol
-403.1 Étendue de l’assurance
-Si plusieurs lieux sont assurés dans la même police, la couverture d’assurance s’applique à toutes les choses assurées de ces lieux.
-403.1.1 Vol simple à l’extérieur
-Les choses assurées dans l’assurance inventaire du ménage sont assurées jusqu’à la somme d’assurance convenue au premier risque contre le vol simple dans l’assurance externe selon l’art.102.2.2.
-La couverture vol simple à l'extérieur vient se rajouter à la couverture vol simple de l'article 110 et enlève la restriction qui ne couvre pas le vol simple à l'extérieur. De ce fait, avec cette couverture complémentaire le vol simple est couvert à l'extérieur - par exemple dans la rue, dans un bar, dans un train.
-Restriction de l’étendue de l’assurance
-Ne sont pas assurés les valeurs pécuniaires et les dommages résultant de la perte ou de l’égarement de choses.
-403.2 Franchise
-La franchise est de CHF 200 par événement, dans la mesure où la police ne prévoit pas d’autre franchise.
-113.2.5 Somme d’assurance pour les objets de 
-remplacement en cas de retard des bagages
-Les frais d’achat d’objets de remplacement dans le cas de la livraison en retard des bagages confiés à un transpor_x0002_teur sont couverts si l’assurance complémentaire supervol est souscrite. La limitation des prestations correspondante est mentionnée à l’art.403.1.2 b).
-403.1.2 Détérioration et pertes d’objets en voyage
-La somme d’assurance convenue au premier risque en cas de supervol est doublée et l’étendue de l’assurance suivante s’applique en plus de la couverture selon l’art.403.1.1 (avec somme d’assurance doublée également) pour l’inventaire du ménage assuré emporté lors d’un voyage si:
-• la destination du voyage d’une personne assurée se situe à plus de 50km à vol d’oiseau de l’adresse du domicile assuré (inventaire du ménage au domicile)
-ou • la personne assurée passe au moins une nuit à l’extérieur de ce domicile.
-La couverture d’assurance est valable dans le monde entier, elle commence lors du départ en voyage après avoir quitté l’appartement et prend fin lors du retour en pénétrant dans l’appartement.
-a) Événements assurés
-Sont assurés la perte ainsi que les détériorations ou les destructions survenant subitement et de façon imprévue, dues à l’action d’une force extérieure violente.
-b) Retard des bagages
-Sont assurés les frais d’acquisition absolument nécessaire d’objets de rechange jusqu’à maximum 30% de la somme d’assurance en cas de retard de livraison des bagages 
-confiés pour être acheminés.
-c) Restriction de l’étendue de l’assurance 
-Sont exclus de l’assurance 
-• les valeurs pécuniaires;
-• les dommages qui sont assurés dans le cadre d’événe_x0002_ments incendie, dommages naturels, vol, dégâts d’eau ou bris de glace;
-• le vol simple à l’extérieur (assuré selon l’art.403.1.1);
-• les dommages causés par des rongeurs et des vermines;
-• appareils de sport, vélos et cyclomoteurs, avec tous leurs accessoires, utilisés en compétition;
-• les appareils de sport dotés de leur propre moteur (à l’exception des cyclomoteurs pour lesquels aucune assurance responsabilité civile n’est légalement pres_x0002_crite);
-• les dommages causés par la pluie, l’eau de la fonte de neige ou de glace qui s’est infiltrée par des lucarnes, des fenêtres et portes ouvertes ou des ouvertures dans le toit, par les murs de nouvelles constructions ou lors de travaux de transformation ou autres travaux dans le bâtiment;
-• les données se trouvant sur des choses assurées comme les photos, les fichiers musicaux ou les logiciels d’applications, par exemple;
-• les dommages causés par des animaux domestiques par rayures, morsures et sécrétions;
-• les blessures ou la mort d’animaux;
-• la fraude, l’abus de confiance ou les détournements;
-• la réalisation forcée en matière de poursuite ou de faillite, ou la confiscation par des organes publics.
-403.2 Franchise
-La franchise est de CHF 200 par événement, dans la mesure où la police ne prévoit pas d’autre franchise.
-Art. 113 Prestations
-113.1 Valeur de remplacement et calcul du dommage
-Pour l’inventaire du ménage, les effets d’hôtes et les objets confiés, le dommage est calculé à partir du montant du remplacement à la valeur à neuf au moment du cas de sinistre (= valeur de remplacement), déduction faite de la valeur des restes. Une valeur d’amateur personnelle n’est pas prise en considération. En cas de dommage partiel, le dommage est calculé à partir des frais de réparation à  concurrence de la valeur de remplacement.
-113.2 Sommes d’assurance et limitations des prestations
-La somme d’assurance constitue la limite d’indemnisation, dans la mesure où certaines limitations de prestations particulières ne sont pas applicables. Pour les dommages relevant du champ d’application de l’assurance des dommages naturels légale, les dispositions légales mentionnées à l’art. 17 s’appliquent.
-Art.404 Perte de clés
-Si le vol simple à l’extérieur, le supervol ou All Risk ont été convenus, la perte de clés est également assurée.
-404.1 Étendue de l’assurance, prestations et franchise
-En cas de perte de clés ou de codes, de cartes de systèmes d’accès électroniques (badge) et d’objets similaires, les frais de modification ou de remplacement des serrures 
-(y compris les serrures provisoires) et des clés correspon_x0002_dantes sur les lieux désignés dans la police sont assurés à concurrence de 50% de la somme d’assurance convenue 
-pour le vol simple à l’extérieur, au maximum toutefois à CHF 4’000. De plus, les dispositions suivantes s’appliquent:
-• le doublement de la somme d’assurance en cas de supervol n’est pas pris en compte,
-• pour All Risk, les prestations sont assurées jusqu’à CHF 4’000.
-Si les frais des serrures de fortune excèdent la somme d’assurance, l’assurance complémentaire «Home Assis_x0002_tance» peut intervenir en complément si elle a été incluse dans le contrat.
-La perte de clés de coffres-forts loués est également assurée dans le même cadre.
-La franchise de l’assurance vol ou All Risk s’applique.
-404.2 Restrictions de l’étendue de l’assurance
-Ne sont pas assurés, les clés, codes, badges etc.des locaux professionnels et des véhicules</t>
   </si>
   <si>
     <t>Art. 403, 404, 113</t>
@@ -1590,6 +1531,85 @@
 La franchise de l’assurance vol ou All Risk s’applique.
 404.2 Restrictions de l’étendue de l’assurance
 Ne sont pas assurés, les clés, codes, badges etc.des locaux professionnels et des véhicules"</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Art.403 Supervol
+403.1 Étendue de l’assurance
+Si plusieurs lieux sont assurés dans la même police, la couverture d’assurance s’applique à toutes les choses assurées de ces lieux.
+403.1.1 Vol simple à l’extérieur
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="5" tint="-0.499984740745262"/>
+        <rFont val="Aptos Narrow"/>
+      </rPr>
+      <t xml:space="preserve">La couverture supervol inclut la couverture du vol à l'extérieur qui signifie en dehors du domicile.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>Les choses assurées dans l’assurance inventaire du ménage sont assurées jusqu’à la somme d’assurance convenue au premier risque contre le vol simple dans l’assurance externe selon l’art.102.2.2.
+La couverture vol simple à l'extérieur vient se rajouter à la couverture vol simple de l'article 110 et enlève la restriction qui ne couvre pas le vol simple à l'extérieur. De ce fait, avec cette couverture complémentaire le vol simple est couvert à l'extérieur - par exemple dans la rue, dans un bar, dans un train.
+Restriction de l’étendue de l’assurance
+Ne sont pas assurés les valeurs pécuniaires et les dommages résultant de la perte ou de l’égarement de choses.
+403.2 Franchise
+La franchise est de CHF 200 par événement, dans la mesure où la police ne prévoit pas d’autre franchise.
+113.2.5 Somme d’assurance pour les objets de 
+remplacement en cas de retard des bagages
+Les frais d’achat d’objets de remplacement dans le cas de la livraison en retard des bagages confiés à un transpor_x0002_teur sont couverts si l’assurance complémentaire supervol est souscrite. La limitation des prestations correspondante est mentionnée à l’art.403.1.2 b).
+403.1.2 Détérioration et pertes d’objets en voyage
+La somme d’assurance convenue au premier risque en cas de supervol est doublée et l’étendue de l’assurance suivante s’applique en plus de la couverture selon l’art.403.1.1 (avec somme d’assurance doublée également) pour l’inventaire du ménage assuré emporté lors d’un voyage si:
+• la destination du voyage d’une personne assurée se situe à plus de 50km à vol d’oiseau de l’adresse du domicile assuré (inventaire du ménage au domicile)
+ou • la personne assurée passe au moins une nuit à l’extérieur de ce domicile.
+La couverture d’assurance est valable dans le monde entier, elle commence lors du départ en voyage après avoir quitté l’appartement et prend fin lors du retour en pénétrant dans l’appartement.
+a) Événements assurés
+Sont assurés la perte ainsi que les détériorations ou les destructions survenant subitement et de façon imprévue, dues à l’action d’une force extérieure violente.
+b) Retard des bagages
+Sont assurés les frais d’acquisition absolument nécessaire d’objets de rechange jusqu’à maximum 30% de la somme d’assurance en cas de retard de livraison des bagages 
+confiés pour être acheminés.
+c) Restriction de l’étendue de l’assurance 
+Sont exclus de l’assurance 
+• les valeurs pécuniaires;
+• les dommages qui sont assurés dans le cadre d’événe_x0002_ments incendie, dommages naturels, vol, dégâts d’eau ou bris de glace;
+• le vol simple à l’extérieur (assuré selon l’art.403.1.1);
+• les dommages causés par des rongeurs et des vermines;
+• appareils de sport, vélos et cyclomoteurs, avec tous leurs accessoires, utilisés en compétition;
+• les appareils de sport dotés de leur propre moteur (à l’exception des cyclomoteurs pour lesquels aucune assurance responsabilité civile n’est légalement pres_x0002_crite);
+• les dommages causés par la pluie, l’eau de la fonte de neige ou de glace qui s’est infiltrée par des lucarnes, des fenêtres et portes ouvertes ou des ouvertures dans le toit, par les murs de nouvelles constructions ou lors de travaux de transformation ou autres travaux dans le bâtiment;
+• les données se trouvant sur des choses assurées comme les photos, les fichiers musicaux ou les logiciels d’applications, par exemple;
+• les dommages causés par des animaux domestiques par rayures, morsures et sécrétions;
+• les blessures ou la mort d’animaux;
+• la fraude, l’abus de confiance ou les détournements;
+• la réalisation forcée en matière de poursuite ou de faillite, ou la confiscation par des organes publics.
+403.2 Franchise
+La franchise est de CHF 200 par événement, dans la mesure où la police ne prévoit pas d’autre franchise.
+Art. 113 Prestations
+113.1 Valeur de remplacement et calcul du dommage
+Pour l’inventaire du ménage, les effets d’hôtes et les objets confiés, le dommage est calculé à partir du montant du remplacement à la valeur à neuf au moment du cas de sinistre (= valeur de remplacement), déduction faite de la valeur des restes. Une valeur d’amateur personnelle n’est pas prise en considération. En cas de dommage partiel, le dommage est calculé à partir des frais de réparation à  concurrence de la valeur de remplacement.
+113.2 Sommes d’assurance et limitations des prestations
+La somme d’assurance constitue la limite d’indemnisation, dans la mesure où certaines limitations de prestations particulières ne sont pas applicables. Pour les dommages relevant du champ d’application de l’assurance des dommages naturels légale, les dispositions légales mentionnées à l’art. 17 s’appliquent.
+Art.404 Perte de clés
+Si le vol simple à l’extérieur, le supervol ou All Risk ont été convenus, la perte de clés est également assurée.
+404.1 Étendue de l’assurance, prestations et franchise
+En cas de perte de clés ou de codes, de cartes de systèmes d’accès électroniques (badge) et d’objets similaires, les frais de modification ou de remplacement des serrures 
+(y compris les serrures provisoires) et des clés correspon_x0002_dantes sur les lieux désignés dans la police sont assurés à concurrence de 50% de la somme d’assurance convenue 
+pour le vol simple à l’extérieur, au maximum toutefois à CHF 4’000. De plus, les dispositions suivantes s’appliquent:
+• le doublement de la somme d’assurance en cas de supervol n’est pas pris en compte,
+• pour All Risk, les prestations sont assurées jusqu’à CHF 4’000.
+Si les frais des serrures de fortune excèdent la somme d’assurance, l’assurance complémentaire «Home Assis_x0002_tance» peut intervenir en complément si elle a été incluse dans le contrat.
+La perte de clés de coffres-forts loués est également assurée dans le même cadre.
+La franchise de l’assurance vol ou All Risk s’applique.
+404.2 Restrictions de l’étendue de l’assurance
+Ne sont pas assurés, les clés, codes, badges etc.des locaux professionnels et des véhicules</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -2031,7 +2051,7 @@
   <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2220,7 +2240,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>8</v>
@@ -2289,7 +2309,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>8</v>
@@ -2358,7 +2378,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C15" s="6" t="s">
         <v>8</v>
@@ -2381,7 +2401,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>8</v>
@@ -2404,7 +2424,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C17" s="6" t="s">
         <v>8</v>
@@ -2427,7 +2447,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>8</v>
@@ -2450,7 +2470,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C19" s="6"/>
       <c r="D19" s="7">
@@ -2487,7 +2507,7 @@
         <v>21</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>37</v>
+        <v>63</v>
       </c>
       <c r="C21" s="6" t="s">
         <v>35</v>
@@ -2499,7 +2519,7 @@
         <v>22</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G21" s="6" t="s">
         <v>10</v>
@@ -2510,7 +2530,7 @@
         <v>22</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C22" s="6" t="s">
         <v>35</v>
@@ -2522,7 +2542,7 @@
         <v>25</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G22" s="6" t="s">
         <v>10</v>
@@ -2533,7 +2553,7 @@
         <v>23</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C23" s="6" t="s">
         <v>35</v>
@@ -2543,7 +2563,7 @@
       </c>
       <c r="E23" s="6"/>
       <c r="F23" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G23" s="6" t="s">
         <v>10</v>
@@ -2554,7 +2574,7 @@
         <v>24</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C24" s="6" t="s">
         <v>35</v>
@@ -2564,7 +2584,7 @@
       </c>
       <c r="E24" s="6"/>
       <c r="F24" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G24" s="6" t="s">
         <v>10</v>
@@ -2575,7 +2595,7 @@
         <v>25</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C25" s="6" t="s">
         <v>35</v>
@@ -2585,7 +2605,7 @@
       </c>
       <c r="E25" s="6"/>
       <c r="F25" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G25" s="6" t="s">
         <v>10</v>
@@ -2596,7 +2616,7 @@
         <v>26</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C26" s="6" t="s">
         <v>35</v>
@@ -2606,7 +2626,7 @@
       </c>
       <c r="E26" s="6"/>
       <c r="F26" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G26" s="6" t="s">
         <v>10</v>
@@ -2617,7 +2637,7 @@
         <v>27</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C27" s="6" t="s">
         <v>35</v>
@@ -2627,7 +2647,7 @@
       </c>
       <c r="E27" s="6"/>
       <c r="F27" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G27" s="6" t="s">
         <v>10</v>
@@ -2638,7 +2658,7 @@
         <v>28</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C28" s="6" t="s">
         <v>35</v>
@@ -2648,7 +2668,7 @@
       </c>
       <c r="E28" s="6"/>
       <c r="F28" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G28" s="6" t="s">
         <v>10</v>
@@ -2659,7 +2679,7 @@
         <v>29</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C29" s="6" t="s">
         <v>35</v>
@@ -2669,7 +2689,7 @@
       </c>
       <c r="E29" s="6"/>
       <c r="F29" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G29" s="6" t="s">
         <v>10</v>
@@ -2680,7 +2700,7 @@
         <v>30</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C30" s="6" t="s">
         <v>35</v>
@@ -2690,7 +2710,7 @@
       </c>
       <c r="E30" s="6"/>
       <c r="F30" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G30" s="6" t="s">
         <v>10</v>
@@ -2701,7 +2721,7 @@
         <v>31</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C31" s="6" t="s">
         <v>35</v>
@@ -2711,7 +2731,7 @@
       </c>
       <c r="E31" s="6"/>
       <c r="F31" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G31" s="6" t="s">
         <v>10</v>
@@ -2722,7 +2742,7 @@
         <v>32</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C32" s="6" t="s">
         <v>35</v>
@@ -2732,7 +2752,7 @@
       </c>
       <c r="E32" s="6"/>
       <c r="F32" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G32" s="6" t="s">
         <v>10</v>
@@ -2743,7 +2763,7 @@
         <v>33</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C33" s="6" t="s">
         <v>35</v>
@@ -2753,7 +2773,7 @@
       </c>
       <c r="E33" s="6"/>
       <c r="F33" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G33" s="6" t="s">
         <v>10</v>
@@ -2764,7 +2784,7 @@
         <v>34</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C34" s="6" t="s">
         <v>35</v>
@@ -2774,7 +2794,7 @@
       </c>
       <c r="E34" s="6"/>
       <c r="F34" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G34" s="6" t="s">
         <v>10</v>
@@ -2782,5 +2802,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>